<commit_message>
Maj labels et liens page contact
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO (1) (1).xlsx
+++ b/Modèle-audit-SEO (1) (1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -60,6 +60,9 @@
 Utiliser les format webp</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Media/Formats/Image_types#webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 accessibilité</t>
   </si>
@@ -79,6 +82,10 @@
     <t xml:space="preserve">utiliser un fond noir pour 
      avoir un bon contraste 
 Avec le fond </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast
+https://www.w3.org/TR/WCAG/#contrast-minimum</t>
   </si>
   <si>
     <t xml:space="preserve">accessibilité</t>
@@ -143,103 +150,16 @@
 Derrière les image</t>
   </si>
   <si>
-    <t xml:space="preserve">Des balise &lt;li&gt; sont utiliser 
-pour crée des espaces </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Des balise &lt;li&gt; sont utiliser 
-pour faire des espaces 
-cela peut créé des soucis 
-d'optimisation ou de 
-validateur W3C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utiliser des propriété 
-comme flexbox ou encore 
-gap pour crée des espace
-entre les éléments </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utiliser des propriétaire 
-comme flexbox ou encore 
-gap pour crée des espace
-entre les éléments </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il ya des class en trop qui 
-Mélange plein d’élément </t>
-  </si>
-  <si>
-    <t xml:space="preserve">il ya des class en trop cela
-crée des erreur quand je 
-veut faire des modifs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">éviter d'utiliser les class
-dans n’importe qu'elle 
-éléments </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retravailler les classes
-Utilisées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mettre les bonnes class 
-pour les images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les images nont pas les 
-bonne classe cela peut 
-inpacté les taille </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faire des bonne class pour
-une page bien structurer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retravailler les classes 
-Utilisées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refaire le responsive design
-pour adapter à tout type 
-d’écran </t>
-  </si>
-  <si>
-    <t xml:space="preserve">le responsive ne sont pas
-adapter pour les écran </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penser au responsive dès 
-la conception, 
-et tester le site à chaque 
-étape du développement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Retester le résponsive et 
-retravailler le 
-Css et 
-les media queries pour 
-     s'assurer de la bonne 
-mise 
-      En page à tous les formats 
-D'écrans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le css est mal structurer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">plusieurs élément son modifier
-avec plusieurs style css</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bien structurer son css </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réorganiser le css et 
-rassembler
- les différents blocs
- Par éléments stylisés </t>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/Img#attributs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respecter les bonnes pratiques et la structuration sémantique du html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des balises &lt;li&gt; utilisées pour créer des espaces, mélanges de classes css, ordre des titres (h1,h2,h3) non respecté, structure non responsive, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réorganiser le code, respecter la sémantique des balises, réorganiser le css, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">Aucun lien mène vers les 
@@ -256,6 +176,18 @@
   <si>
     <t xml:space="preserve">Ajouté les bon lien pour 
 la redirection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimisation des ressources externes (css/js)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renseigner informations d’accessibilité et métadonnées (title, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balises Aria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Éviter pratiques « black hat » : keywords, annuaires, etc.</t>
   </si>
 </sst>
 </file>
@@ -265,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -306,7 +238,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -318,8 +250,22 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +276,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -367,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -384,7 +342,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,20 +358,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -479,7 +441,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -489,21 +451,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.09765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.11328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="74.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.6"/>
   </cols>
   <sheetData>
@@ -563,175 +525,134 @@
       <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>11</v>
+      <c r="A3" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="9" t="s">
         <v>15</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>16</v>
+      <c r="A4" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
+      <c r="A5" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>21</v>
+      <c r="A6" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>21</v>
+    <row r="7" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>33</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>21</v>
+    <row r="8" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="7" t="s">
+    <row r="9" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="9" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="7" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1718,10 +1639,11 @@
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>